<commit_message>
new time series test data inside the Excel to test the method that adjust the profile data to the opf settings
</commit_message>
<xml_diff>
--- a/pyensys/tests/excel/time_series_pandapower_attest_format.xlsx
+++ b/pyensys/tests/excel/time_series_pandapower_attest_format.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7116"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7116" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="2">
   <si>
     <t>P</t>
   </si>
@@ -349,8 +350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -414,4 +415,99 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>